<commit_message>
Update 0524 meeting discussion
</commit_message>
<xml_diff>
--- a/data/test/test_result.xlsx
+++ b/data/test/test_result.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JustinHsu\Desktop\math-friday\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Lee\Desktop\RAG_Search_Weights\data\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F674CA88-CAF4-4BC2-AF62-870484145F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB860C9-41D4-448B-9B2E-F4966BD12C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="alpha 0.9" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -28,18 +28,6 @@
     <t>答案</t>
   </si>
   <si>
-    <t>檢索結果_0.1</t>
-  </si>
-  <si>
-    <t>GPT_結果_0.1</t>
-  </si>
-  <si>
-    <t>檢索驗證_0.1</t>
-  </si>
-  <si>
-    <t>答案驗證_0.1</t>
-  </si>
-  <si>
     <t>女老師 蔡炎龍 學生</t>
   </si>
   <si>
@@ -84,6 +72,22 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>檢索結果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPT_結果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>檢索驗證</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>答案驗證</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -461,13 +465,17 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" customWidth="1"/>
     <col min="3" max="3" width="33.59765625" customWidth="1"/>
     <col min="4" max="4" width="29.3984375" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" customWidth="1"/>
+    <col min="6" max="6" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -478,76 +486,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>